<commit_message>
Adding Mistral AI cleaning functionality
</commit_message>
<xml_diff>
--- a/BookToValidate02.xlsx
+++ b/BookToValidate02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChaibgalliCl_3jx4l8\OneDrive\Documents\githubProjects\validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/githubProjects/validator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE77D52-8FC8-46A4-AB66-33C9950B804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{BEE77D52-8FC8-46A4-AB66-33C9950B804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8051D2DC-1E2A-4F6B-85E6-97E2862D111D}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
+    <workbookView xWindow="1635" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Book_01" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
   <si>
     <t>US/Canada</t>
   </si>
@@ -289,6 +289,72 @@
   </si>
   <si>
     <t>Tegucigalpa</t>
+  </si>
+  <si>
+    <t>A048</t>
+  </si>
+  <si>
+    <t>A049</t>
+  </si>
+  <si>
+    <t>A050</t>
+  </si>
+  <si>
+    <t>A051</t>
+  </si>
+  <si>
+    <t>A052</t>
+  </si>
+  <si>
+    <t>A053</t>
+  </si>
+  <si>
+    <t>A054</t>
+  </si>
+  <si>
+    <t>A055</t>
+  </si>
+  <si>
+    <t>A056</t>
+  </si>
+  <si>
+    <t>A057</t>
+  </si>
+  <si>
+    <t>A058</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Aubervilliers</t>
+  </si>
+  <si>
+    <t>Koper</t>
+  </si>
+  <si>
+    <t>Kkorea</t>
+  </si>
+  <si>
+    <t>Hawaï</t>
+  </si>
+  <si>
+    <t>Norge</t>
+  </si>
+  <si>
+    <t>Den russiske føderasjon</t>
+  </si>
+  <si>
+    <t>Новая Зеландия</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>Prtgal</t>
+  </si>
+  <si>
+    <t>Zimbabyoue</t>
   </si>
 </sst>
 </file>
@@ -723,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5218D5-9F32-4A80-8491-65FEDECEA1DF}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1116,6 +1182,94 @@
       </c>
       <c r="B48" s="2" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding app03.js for country match
</commit_message>
<xml_diff>
--- a/BookToValidate02.xlsx
+++ b/BookToValidate02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/githubProjects/validator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{BEE77D52-8FC8-46A4-AB66-33C9950B804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8051D2DC-1E2A-4F6B-85E6-97E2862D111D}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{BEE77D52-8FC8-46A4-AB66-33C9950B804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF080224-846C-4DFB-A842-DCA98EC8A394}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
+    <workbookView xWindow="8175" yWindow="4680" windowWidth="21600" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Book_01" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
   <si>
     <t>US/Canada</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Zimbabyoue</t>
+  </si>
+  <si>
+    <t>Country of Origin</t>
   </si>
 </sst>
 </file>
@@ -393,6 +396,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -792,7 +796,7 @@
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -805,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>